<commit_message>
add description column to facilitate leave application from previous months.
</commit_message>
<xml_diff>
--- a/test/digio_leave.xlsx
+++ b/test/digio_leave.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t xml:space="preserve">Project Resource Name</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">Organization: Organization Name</t>
   </si>
   <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
     <t xml:space="preserve">Syril Sadasivan</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">DigIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave request 28/03/2020</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Leave</t>
@@ -65,7 +71,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -99,6 +105,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,7 +162,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -174,6 +185,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -195,13 +210,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="1" style="1" width="11.42"/>
   </cols>
@@ -225,10 +240,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>43949</v>
@@ -238,15 +256,18 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>43949</v>
@@ -256,15 +277,18 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>43949</v>
@@ -274,15 +298,18 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
+      <c r="G4" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>43949</v>
@@ -292,10 +319,13 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>